<commit_message>
prep files to draft EML xml for publication datasets
</commit_message>
<xml_diff>
--- a/round2_metareview/publish/internaluse/ecolofES_EMLmetadata_prep.xlsx
+++ b/round2_metareview/publish/internaluse/ecolofES_EMLmetadata_prep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scarlet/github/kremeny_analyses/round2_metareview/publish/internaluse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD196988-C41A-E943-9C00-108E93A442C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA96F3D-D3AB-6647-AAC1-927AE6DE00A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-4260" windowWidth="27200" windowHeight="14860" activeTab="2" xr2:uid="{46313B9D-46D1-0F4C-9AF2-2DB58079C1CD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
   <definedNames>
     <definedName name="dataTable">[1]DataSetEntities!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="243">
   <si>
     <t>title</t>
   </si>
@@ -185,553 +185,595 @@
     <t>Laura</t>
   </si>
   <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>Julie</t>
+  </si>
+  <si>
+    <t>Dragone</t>
+  </si>
+  <si>
+    <t>Grabenstein</t>
+  </si>
+  <si>
+    <t>Kathryn</t>
+  </si>
+  <si>
+    <t>Jech</t>
+  </si>
+  <si>
+    <t>Sierra</t>
+  </si>
+  <si>
+    <t>de Silva</t>
+  </si>
+  <si>
+    <t>Isabel</t>
+  </si>
+  <si>
+    <t>Karban</t>
+  </si>
+  <si>
+    <t>Claire</t>
+  </si>
+  <si>
+    <t>Brigham</t>
+  </si>
+  <si>
+    <t>Laurel</t>
+  </si>
+  <si>
+    <t>McDevitt-Galles</t>
+  </si>
+  <si>
+    <t>Travis</t>
+  </si>
+  <si>
+    <t>Spiers</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Korpita</t>
+  </si>
+  <si>
+    <t>Nicholas</t>
+  </si>
+  <si>
+    <t>nicholas.dragone@colorado.edu</t>
+  </si>
+  <si>
+    <t>caitlin.t.white@colorado.edu</t>
+  </si>
+  <si>
+    <t>isabel.desilva@colorado.edu</t>
+  </si>
+  <si>
+    <t>grant.vagle@colorado.edu</t>
+  </si>
+  <si>
+    <t>kathryn.grabenstein@colorado.edu</t>
+  </si>
+  <si>
+    <t>timothy.korpita@colorado.edu</t>
+  </si>
+  <si>
+    <t>Timothy</t>
+  </si>
+  <si>
+    <t>laurel.brigham@colorado.edu</t>
+  </si>
+  <si>
+    <t>claire.karban@colorado.edu</t>
+  </si>
+  <si>
+    <t>aislyn.keyes@colorado.edu</t>
+  </si>
+  <si>
+    <t>sierra.jech@colorado.edu</t>
+  </si>
+  <si>
+    <t>anna.spiers@colorado.edu</t>
+  </si>
+  <si>
+    <t>laura.dee@colorado.edu</t>
+  </si>
+  <si>
+    <t>tmcdevittgalles@gmail.com</t>
+  </si>
+  <si>
+    <t>Larson</t>
+  </si>
+  <si>
+    <t>julie.e.larson@colorado.edu</t>
+  </si>
+  <si>
+    <t>organizationName</t>
+  </si>
+  <si>
+    <t>RoleType</t>
+  </si>
+  <si>
+    <t>pointOfContact, author</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>metadataProvider, author</t>
+  </si>
+  <si>
+    <t>salutation</t>
+  </si>
+  <si>
+    <t>Dr.</t>
+  </si>
+  <si>
+    <t>Mr.</t>
+  </si>
+  <si>
+    <t>Ms.</t>
+  </si>
+  <si>
+    <t>Title of study</t>
+  </si>
+  <si>
+    <t>Full list of study authors</t>
+  </si>
+  <si>
+    <t>Year study published</t>
+  </si>
+  <si>
+    <t>Anonymized reviewer identity</t>
+  </si>
+  <si>
+    <t>Whether study was double reviewed or not</t>
+  </si>
+  <si>
+    <t>Question abbreviation</t>
+  </si>
+  <si>
+    <t>Question number</t>
+  </si>
+  <si>
+    <t>Full question description</t>
+  </si>
+  <si>
+    <t>Answer as entered by reviewer</t>
+  </si>
+  <si>
+    <t>Quality controlled answer prepared for data synthesis</t>
+  </si>
+  <si>
+    <t>Binned driver variable</t>
+  </si>
+  <si>
+    <t>Driver group as selected by reviewer</t>
+  </si>
+  <si>
+    <t>Quality controlled driver group</t>
+  </si>
+  <si>
+    <t>Land use land cover adjusted driver group</t>
+  </si>
+  <si>
+    <t>Ecosystem service</t>
+  </si>
+  <si>
+    <t>Ecosystem service category</t>
+  </si>
+  <si>
+    <t>Whether study only considered land use land cover drivers</t>
+  </si>
+  <si>
+    <t>Journal where study published</t>
+  </si>
+  <si>
+    <t>YYYY</t>
+  </si>
+  <si>
+    <t>attributeLabel</t>
+  </si>
+  <si>
+    <t>storageType</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>dateTime</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Full authors</t>
+  </si>
+  <si>
+    <t>Publication year</t>
+  </si>
+  <si>
+    <t>Publication source</t>
+  </si>
+  <si>
+    <t>Review stage</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>Double reviewed</t>
+  </si>
+  <si>
+    <t>Reviewer notes</t>
+  </si>
+  <si>
+    <t>Outside reviewer</t>
+  </si>
+  <si>
+    <t>Outside reviewer notes</t>
+  </si>
+  <si>
+    <t>Exclusion ID</t>
+  </si>
+  <si>
+    <t>Exclusion reason</t>
+  </si>
+  <si>
+    <t>Full question</t>
+  </si>
+  <si>
+    <t>Raw answer</t>
+  </si>
+  <si>
+    <t>Clean answer</t>
+  </si>
+  <si>
+    <t>Variable number</t>
+  </si>
+  <si>
+    <t>Clean answer binned</t>
+  </si>
+  <si>
+    <t>Raw group</t>
+  </si>
+  <si>
+    <t>Clean group</t>
+  </si>
+  <si>
+    <t>Land Use Land Cover group</t>
+  </si>
+  <si>
+    <t>Survey order</t>
+  </si>
+  <si>
+    <t>QA note</t>
+  </si>
+  <si>
+    <t>LULC recode note</t>
+  </si>
+  <si>
+    <t>Only LULC</t>
+  </si>
+  <si>
+    <t>Notes on land use land cover adjustment applied</t>
+  </si>
+  <si>
+    <t>Abbreviation</t>
+  </si>
+  <si>
+    <t>Question ID</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>entityType</t>
+  </si>
+  <si>
+    <t>entityName</t>
+  </si>
+  <si>
+    <t>entitydescription</t>
+  </si>
+  <si>
+    <t>entityfilename</t>
+  </si>
+  <si>
+    <t>maintenance</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>ecolofES_excludedpapers.csv</t>
+  </si>
+  <si>
+    <t>ecolofES_extracted_data.csv</t>
+  </si>
+  <si>
+    <t>dataTable</t>
+  </si>
+  <si>
+    <t>Ecology of ecosystem services systematic map: extracted meta-data</t>
+  </si>
+  <si>
+    <t>Ecology of ecosystem services systematic map: excluded articles</t>
+  </si>
+  <si>
+    <t>EcolofES extracted meta-data</t>
+  </si>
+  <si>
+    <t>shortname</t>
+  </si>
+  <si>
+    <t>EcolofES_extracted</t>
+  </si>
+  <si>
+    <t>EcolofES_excluded</t>
+  </si>
+  <si>
+    <t>Extracted meta-data from studies retained after abstract and full-text screening stages, with study citation information</t>
+  </si>
+  <si>
+    <t>EcolofES excluded articles</t>
+  </si>
+  <si>
+    <t>All studies excluded at abstract or full-text screening stages, with reason for exclusion and ctudy citation information</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>Count of unique variables study considered, per ecosystem service category, per response or driver category</t>
+  </si>
+  <si>
+    <t>Whether answer is final answer used for data synthesis (all single-reviewed answers, consolidated and reconciled double-reviewed answers) or individual answer for double reviewed studies</t>
+  </si>
+  <si>
+    <t>Qualtrics-assigned unique question ID</t>
+  </si>
+  <si>
+    <t>Order of question and sub-question appearance in survey; unique ID alternative to Qualitrics question ID field</t>
+  </si>
+  <si>
+    <t>Notes on any quality control action applied to raw answer or raw driver group</t>
+  </si>
+  <si>
+    <t>Whether study was excluded at title and abstract screening stage or full-text screening stage</t>
+  </si>
+  <si>
+    <t>Reviewer notes on exclusion</t>
+  </si>
+  <si>
+    <t>Anonymized identity of third party reviewer when needed</t>
+  </si>
+  <si>
+    <t>Third party reviewer notes on exclusion</t>
+  </si>
+  <si>
+    <t>Unique code for exclusion</t>
+  </si>
+  <si>
+    <t>Primary reason for exclusion</t>
+  </si>
+  <si>
+    <t>Full exclusion criterion question</t>
+  </si>
+  <si>
+    <t>entityname</t>
+  </si>
+  <si>
+    <t>Department of Ecology and Evolutionary Biology, University of Colorado Boulder</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>HabCreate</t>
+  </si>
+  <si>
+    <t>Habitat creation and maintenance</t>
+  </si>
+  <si>
+    <t>Pollination</t>
+  </si>
+  <si>
+    <t>Pollination and dispersal of seeds and other propagules</t>
+  </si>
+  <si>
+    <t>AQReg</t>
+  </si>
+  <si>
+    <t>Regulation of air quality</t>
+  </si>
+  <si>
+    <t>ClimReg</t>
+  </si>
+  <si>
+    <t>Regulation of climate</t>
+  </si>
+  <si>
+    <t>OceanReg</t>
+  </si>
+  <si>
+    <t>Regulation of ocean acidification</t>
+  </si>
+  <si>
+    <t>freshWQReg</t>
+  </si>
+  <si>
+    <t>Regulation of freshwater quantity, location and timing</t>
+  </si>
+  <si>
+    <t>coastWQReg</t>
+  </si>
+  <si>
+    <t>Regulation of freshwater and coastal water quality</t>
+  </si>
+  <si>
+    <t>SoilProtect</t>
+  </si>
+  <si>
+    <t>Formation, protection and decontamination of soils and sediments</t>
+  </si>
+  <si>
+    <t>Hazards</t>
+  </si>
+  <si>
+    <t>Regulation of hazards and extreme events</t>
+  </si>
+  <si>
+    <t>PestPath</t>
+  </si>
+  <si>
+    <t>Regulation of detrimental organisms and biological processes</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Food and feed</t>
+  </si>
+  <si>
+    <t>Materials</t>
+  </si>
+  <si>
+    <t>MedGen</t>
+  </si>
+  <si>
+    <t>Medicinal, biochemical and genetic resources</t>
+  </si>
+  <si>
+    <t>MaintainOpts</t>
+  </si>
+  <si>
+    <t>Maintenance of options</t>
+  </si>
+  <si>
+    <t>CulturePsych</t>
+  </si>
+  <si>
+    <t>Physical and psychological experiences</t>
+  </si>
+  <si>
+    <t>Materials, companionship and labor</t>
+  </si>
+  <si>
+    <t>col_classes</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>factor</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
     <t>0000-0003-0471-1371</t>
   </si>
   <si>
+    <t>0000-0003-0599-3059</t>
+  </si>
+  <si>
     <t>0000-0001-8723-3568</t>
   </si>
   <si>
+    <t>0000-0001-7968-916X</t>
+  </si>
+  <si>
+    <t>0000-0002-4929-5431</t>
+  </si>
+  <si>
+    <t>0000-0003-3517-1072</t>
+  </si>
+  <si>
     <t>0000-0002-1323-1735</t>
   </si>
   <si>
-    <t>0000-0003-0599-3059</t>
-  </si>
-  <si>
-    <t>order</t>
-  </si>
-  <si>
-    <t>Julie</t>
-  </si>
-  <si>
-    <t>Dragone</t>
-  </si>
-  <si>
-    <t>Grabenstein</t>
-  </si>
-  <si>
-    <t>Kathryn</t>
-  </si>
-  <si>
-    <t>Jech</t>
-  </si>
-  <si>
-    <t>Sierra</t>
-  </si>
-  <si>
-    <t>de Silva</t>
-  </si>
-  <si>
-    <t>Isabel</t>
-  </si>
-  <si>
-    <t>Karban</t>
-  </si>
-  <si>
-    <t>Claire</t>
-  </si>
-  <si>
-    <t>Brigham</t>
-  </si>
-  <si>
-    <t>Laurel</t>
-  </si>
-  <si>
-    <t>McDevitt-Galles</t>
-  </si>
-  <si>
-    <t>Travis</t>
-  </si>
-  <si>
-    <t>Spiers</t>
-  </si>
-  <si>
-    <t>Anna</t>
-  </si>
-  <si>
-    <t>Korpita</t>
+    <t>0000-0002-8983-6482</t>
   </si>
   <si>
     <t>0000-0003-4725-3008</t>
   </si>
   <si>
-    <t>0000-0002-4929-5431</t>
-  </si>
-  <si>
-    <t>0000-0003-3517-1072</t>
+    <t>0000-0001-8852-0665</t>
+  </si>
+  <si>
+    <t>0000-0001-5480-7633</t>
   </si>
   <si>
     <t>0000-0001-5592-9165</t>
   </si>
   <si>
-    <t>0000-0001-5480-7633</t>
-  </si>
-  <si>
-    <t>0000-0002-8983-6482</t>
-  </si>
-  <si>
-    <t>Nicholas</t>
-  </si>
-  <si>
-    <t>nicholas.dragone@colorado.edu</t>
-  </si>
-  <si>
-    <t>caitlin.t.white@colorado.edu</t>
-  </si>
-  <si>
-    <t>isabel.desilva@colorado.edu</t>
-  </si>
-  <si>
-    <t>grant.vagle@colorado.edu</t>
-  </si>
-  <si>
-    <t>kathryn.grabenstein@colorado.edu</t>
-  </si>
-  <si>
-    <t>timothy.korpita@colorado.edu</t>
-  </si>
-  <si>
-    <t>Timothy</t>
-  </si>
-  <si>
-    <t>laurel.brigham@colorado.edu</t>
-  </si>
-  <si>
-    <t>claire.karban@colorado.edu</t>
-  </si>
-  <si>
-    <t>aislyn.keyes@colorado.edu</t>
-  </si>
-  <si>
-    <t>sierra.jech@colorado.edu</t>
-  </si>
-  <si>
-    <t>anna.spiers@colorado.edu</t>
-  </si>
-  <si>
-    <t>laura.dee@colorado.edu</t>
-  </si>
-  <si>
-    <t>tmcdevittgalles@gmail.com</t>
-  </si>
-  <si>
-    <t>0000-0001-8852-0665</t>
-  </si>
-  <si>
-    <t>0000-0001-7968-916X</t>
-  </si>
-  <si>
-    <t>Larson</t>
-  </si>
-  <si>
-    <t>julie.e.larson@colorado.edu</t>
-  </si>
-  <si>
     <t>0000-0002-6157-031X</t>
   </si>
   <si>
-    <t>organizationName</t>
-  </si>
-  <si>
-    <t>RoleType</t>
-  </si>
-  <si>
-    <t>pointOfContact, author</t>
-  </si>
-  <si>
-    <t>author</t>
-  </si>
-  <si>
-    <t>metadataProvider, author</t>
-  </si>
-  <si>
-    <t>salutation</t>
-  </si>
-  <si>
-    <t>Dr.</t>
-  </si>
-  <si>
-    <t>Mr.</t>
-  </si>
-  <si>
-    <t>Ms.</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>Title of study</t>
-  </si>
-  <si>
-    <t>Full list of study authors</t>
-  </si>
-  <si>
-    <t>Year study published</t>
-  </si>
-  <si>
-    <t>Anonymized reviewer identity</t>
-  </si>
-  <si>
-    <t>Whether study was double reviewed or not</t>
-  </si>
-  <si>
-    <t>Question abbreviation</t>
-  </si>
-  <si>
-    <t>Question number</t>
-  </si>
-  <si>
-    <t>Full question description</t>
-  </si>
-  <si>
-    <t>Answer as entered by reviewer</t>
-  </si>
-  <si>
-    <t>Quality controlled answer prepared for data synthesis</t>
-  </si>
-  <si>
-    <t>Binned driver variable</t>
-  </si>
-  <si>
-    <t>Driver group as selected by reviewer</t>
-  </si>
-  <si>
-    <t>Quality controlled driver group</t>
-  </si>
-  <si>
-    <t>Land use land cover adjusted driver group</t>
-  </si>
-  <si>
-    <t>Ecosystem service</t>
-  </si>
-  <si>
-    <t>Ecosystem service category</t>
-  </si>
-  <si>
-    <t>Whether study only considered land use land cover drivers</t>
-  </si>
-  <si>
-    <t>Journal where study published</t>
-  </si>
-  <si>
-    <t>YYYY</t>
-  </si>
-  <si>
-    <t>attributeLabel</t>
-  </si>
-  <si>
-    <t>storageType</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>double</t>
-  </si>
-  <si>
-    <t>dateTime</t>
-  </si>
-  <si>
-    <t>boolean</t>
-  </si>
-  <si>
-    <t>decimal</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Full authors</t>
-  </si>
-  <si>
-    <t>Publication year</t>
-  </si>
-  <si>
-    <t>Publication source</t>
-  </si>
-  <si>
-    <t>Review stage</t>
-  </si>
-  <si>
-    <t>Reviewer</t>
-  </si>
-  <si>
-    <t>Double reviewed</t>
-  </si>
-  <si>
-    <t>Reviewer notes</t>
-  </si>
-  <si>
-    <t>Outside reviewer</t>
-  </si>
-  <si>
-    <t>Outside reviewer notes</t>
-  </si>
-  <si>
-    <t>Exclusion ID</t>
-  </si>
-  <si>
-    <t>Exclusion reason</t>
-  </si>
-  <si>
-    <t>Full question</t>
-  </si>
-  <si>
-    <t>Raw answer</t>
-  </si>
-  <si>
-    <t>Clean answer</t>
-  </si>
-  <si>
-    <t>Variable number</t>
-  </si>
-  <si>
-    <t>Clean answer binned</t>
-  </si>
-  <si>
-    <t>Raw group</t>
-  </si>
-  <si>
-    <t>Clean group</t>
-  </si>
-  <si>
-    <t>Land Use Land Cover group</t>
-  </si>
-  <si>
-    <t>Survey order</t>
-  </si>
-  <si>
-    <t>QA note</t>
-  </si>
-  <si>
-    <t>LULC recode note</t>
-  </si>
-  <si>
-    <t>Only LULC</t>
-  </si>
-  <si>
-    <t>Notes on land use land cover adjustment applied</t>
-  </si>
-  <si>
-    <t>Abbreviation</t>
-  </si>
-  <si>
-    <t>Question ID</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>entityType</t>
-  </si>
-  <si>
-    <t>entityName</t>
-  </si>
-  <si>
-    <t>entitydescription</t>
-  </si>
-  <si>
-    <t>entityfilename</t>
-  </si>
-  <si>
-    <t>maintenance</t>
-  </si>
-  <si>
-    <t>complete</t>
-  </si>
-  <si>
-    <t>ecolofES_excludedpapers.csv</t>
-  </si>
-  <si>
-    <t>ecolofES_extracted_data.csv</t>
-  </si>
-  <si>
-    <t>dataTable</t>
-  </si>
-  <si>
-    <t>Ecology of ecosystem services systematic map: extracted meta-data</t>
-  </si>
-  <si>
-    <t>Ecology of ecosystem services systematic map: excluded articles</t>
-  </si>
-  <si>
-    <t>EcolofES extracted meta-data</t>
-  </si>
-  <si>
-    <t>shortname</t>
-  </si>
-  <si>
-    <t>EcolofES_extracted</t>
-  </si>
-  <si>
-    <t>EcolofES_excluded</t>
-  </si>
-  <si>
-    <t>Extracted meta-data from studies retained after abstract and full-text screening stages, with study citation information</t>
-  </si>
-  <si>
-    <t>EcolofES excluded articles</t>
-  </si>
-  <si>
-    <t>All studies excluded at abstract or full-text screening stages, with reason for exclusion and ctudy citation information</t>
-  </si>
-  <si>
-    <t>real</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>Count of unique variables study considered, per ecosystem service category, per response or driver category</t>
-  </si>
-  <si>
-    <t>Whether answer is final answer used for data synthesis (all single-reviewed answers, consolidated and reconciled double-reviewed answers) or individual answer for double reviewed studies</t>
-  </si>
-  <si>
-    <t>Qualtrics-assigned unique question ID</t>
-  </si>
-  <si>
-    <t>Order of question and sub-question appearance in survey; unique ID alternative to Qualitrics question ID field</t>
-  </si>
-  <si>
-    <t>Notes on any quality control action applied to raw answer or raw driver group</t>
-  </si>
-  <si>
-    <t>Whether study was excluded at title and abstract screening stage or full-text screening stage</t>
-  </si>
-  <si>
-    <t>Reviewer notes on exclusion</t>
-  </si>
-  <si>
-    <t>Anonymized identity of third party reviewer when needed</t>
-  </si>
-  <si>
-    <t>Third party reviewer notes on exclusion</t>
-  </si>
-  <si>
-    <t>Unique code for exclusion</t>
-  </si>
-  <si>
-    <t>Primary reason for exclusion</t>
-  </si>
-  <si>
-    <t>Full exclusion criterion question</t>
-  </si>
-  <si>
-    <t>entityname</t>
-  </si>
-  <si>
-    <t>Department of Ecology and Evolutionary Biology, University of Colorado Boulder</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>HabCreate</t>
-  </si>
-  <si>
-    <t>Habitat creation and maintenance</t>
-  </si>
-  <si>
-    <t>Pollination</t>
-  </si>
-  <si>
-    <t>Pollination and dispersal of seeds and other propagules</t>
-  </si>
-  <si>
-    <t>AQReg</t>
-  </si>
-  <si>
-    <t>Regulation of air quality</t>
-  </si>
-  <si>
-    <t>ClimReg</t>
-  </si>
-  <si>
-    <t>Regulation of climate</t>
-  </si>
-  <si>
-    <t>OceanReg</t>
-  </si>
-  <si>
-    <t>Regulation of ocean acidification</t>
-  </si>
-  <si>
-    <t>freshWQReg</t>
-  </si>
-  <si>
-    <t>Regulation of freshwater quantity, location and timing</t>
-  </si>
-  <si>
-    <t>coastWQReg</t>
-  </si>
-  <si>
-    <t>Regulation of freshwater and coastal water quality</t>
-  </si>
-  <si>
-    <t>SoilProtect</t>
-  </si>
-  <si>
-    <t>Formation, protection and decontamination of soils and sediments</t>
-  </si>
-  <si>
-    <t>Hazards</t>
-  </si>
-  <si>
-    <t>Regulation of hazards and extreme events</t>
-  </si>
-  <si>
-    <t>PestPath</t>
-  </si>
-  <si>
-    <t>Regulation of detrimental organisms and biological processes</t>
-  </si>
-  <si>
-    <t>Energy</t>
-  </si>
-  <si>
-    <t>Food</t>
-  </si>
-  <si>
-    <t>Food and feed</t>
-  </si>
-  <si>
-    <t>Materials</t>
-  </si>
-  <si>
-    <t>MedGen</t>
-  </si>
-  <si>
-    <t>Medicinal, biochemical and genetic resources</t>
-  </si>
-  <si>
-    <t>MaintainOpts</t>
-  </si>
-  <si>
-    <t>Maintenance of options</t>
-  </si>
-  <si>
-    <t>CulturePsych</t>
-  </si>
-  <si>
-    <t>Physical and psychological experiences</t>
-  </si>
-  <si>
-    <t>Materials, companionship and labor</t>
-  </si>
-  <si>
-    <t>col_classes</t>
-  </si>
-  <si>
-    <t>character</t>
-  </si>
-  <si>
-    <t>numeric</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>factor</t>
+    <t>any text</t>
+  </si>
+  <si>
+    <t>convention: "Q"[question number, 1-18]</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>Biotic</t>
+  </si>
+  <si>
+    <t>LU_LC</t>
+  </si>
+  <si>
+    <t>Abiotic driver type</t>
+  </si>
+  <si>
+    <t>Anthropogenic driver type</t>
+  </si>
+  <si>
+    <t>Biotic driver type</t>
+  </si>
+  <si>
+    <t>Land use land cover driver type</t>
+  </si>
+  <si>
+    <t>Title and abstract screening stage</t>
+  </si>
+  <si>
+    <t>TRUE or FALSE</t>
+  </si>
+  <si>
+    <t>Full-text screening stage</t>
+  </si>
+  <si>
+    <t>"individual" or "final"</t>
   </si>
 </sst>
 </file>
@@ -1193,32 +1235,32 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="C1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C3" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1247,59 +1289,59 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="C1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="E1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="F1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="E2" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="F2" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="E3" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="F3" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1309,907 +1351,988 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80FC3E4-36C8-D147-B3F4-F90F89CECDA0}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="58.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" customWidth="1"/>
-    <col min="5" max="6" width="43.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="7" width="43.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="C1" t="s">
         <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>30</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>224</v>
+        <v>32</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="H1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>33</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>227</v>
+        <v>92</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="H4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="I4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B6" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B8" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>225</v>
+        <v>242</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B9" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B10" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B11" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B12" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B13" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B14" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B15" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>226</v>
+        <v>164</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="I15" t="s">
-        <v>177</v>
+        <v>212</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="J15" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+      <c r="K15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B16" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B17" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C17" t="s">
         <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>225</v>
+        <v>101</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B18" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C18" t="s">
         <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>225</v>
+        <v>102</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B19" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C19" t="s">
         <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>225</v>
+        <v>103</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B20" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C20" t="s">
         <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>228</v>
+        <v>105</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B21" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C21" t="s">
         <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>226</v>
+        <v>167</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="I21" t="s">
-        <v>177</v>
+        <v>212</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="J21" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+      <c r="K21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B22" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C22" t="s">
         <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B23" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C23" t="s">
         <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B24" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
       </c>
       <c r="D24" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B25" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B26" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B27" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>227</v>
+        <v>92</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="H27" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="I27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B28" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B29" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>225</v>
+        <v>169</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B30" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C30" t="s">
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B31" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B32" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B33" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B34" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
       </c>
       <c r="D34" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B35" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C35" t="s">
         <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="G35" t="s">
-        <v>126</v>
-      </c>
-      <c r="I35" t="s">
-        <v>177</v>
+        <v>173</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="H35" t="s">
+        <v>112</v>
       </c>
       <c r="J35" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+      <c r="K35" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B36" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
       </c>
       <c r="D36" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="G36" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="H36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B37" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="G37" t="s">
-        <v>125</v>
+        <v>229</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="H37" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2219,10 +2342,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{144E29C4-CAE2-414A-8CDA-B25D6576CD5F}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2230,7 +2353,7 @@
     <col min="1" max="1" width="62.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.83203125" style="4"/>
     <col min="3" max="3" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="4"/>
+    <col min="4" max="4" width="11.5" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="8.83203125" style="4"/>
   </cols>
@@ -2240,13 +2363,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>32</v>
@@ -2254,279 +2377,483 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>222</v>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28" t="s">
+        <v>160</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>154</v>
+      </c>
+      <c r="B29" t="s">
+        <v>160</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="4">
+        <v>2</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B1048576" xr:uid="{DCE2CE26-4F2D-A845-9D00-DC74EF0A4F3D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28:B1048576" xr:uid="{DCE2CE26-4F2D-A845-9D00-DC74EF0A4F3D}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -2539,7 +2866,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2547,16 +2874,16 @@
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
     <col min="8" max="8" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
         <v>35</v>
@@ -2568,13 +2895,13 @@
         <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="G1" t="s">
-        <v>103</v>
+        <v>215</v>
       </c>
       <c r="H1" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -2582,7 +2909,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -2591,16 +2918,16 @@
         <v>45</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>216</v>
       </c>
       <c r="H2" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -2608,7 +2935,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
         <v>38</v>
@@ -2617,16 +2944,16 @@
         <v>44</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="F3" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>217</v>
       </c>
       <c r="H3" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2634,7 +2961,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
@@ -2643,16 +2970,16 @@
         <v>43</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="F4" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="G4" t="s">
-        <v>47</v>
+        <v>218</v>
       </c>
       <c r="H4" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -2660,25 +2987,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="F5" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="G5" t="s">
-        <v>90</v>
+        <v>219</v>
       </c>
       <c r="H5" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -2686,7 +3013,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
         <v>41</v>
@@ -2695,16 +3022,16 @@
         <v>42</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" t="s">
+        <v>177</v>
+      </c>
+      <c r="G6" t="s">
+        <v>222</v>
+      </c>
+      <c r="H6" t="s">
         <v>84</v>
-      </c>
-      <c r="F6" t="s">
-        <v>191</v>
-      </c>
-      <c r="G6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -2712,25 +3039,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>223</v>
       </c>
       <c r="H7" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -2738,25 +3065,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F8" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="G8" t="s">
-        <v>68</v>
+        <v>224</v>
       </c>
       <c r="H8" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -2764,25 +3091,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F9" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="G9" t="s">
-        <v>89</v>
+        <v>225</v>
       </c>
       <c r="H9" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -2790,25 +3117,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="F10" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="G10" t="s">
-        <v>72</v>
+        <v>226</v>
       </c>
       <c r="H10" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -2816,25 +3143,25 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="F11" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="G11" t="s">
-        <v>71</v>
+        <v>227</v>
       </c>
       <c r="H11" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -2842,25 +3169,25 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F12" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="G12" t="s">
-        <v>93</v>
+        <v>228</v>
       </c>
       <c r="H12" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -2868,22 +3195,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F13" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="H13" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -2891,25 +3218,25 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="F14" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>220</v>
       </c>
       <c r="H14" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -2917,25 +3244,25 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F15" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="G15" t="s">
-        <v>70</v>
+        <v>221</v>
       </c>
       <c r="H15" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>